<commit_message>
mission page integration in progress
</commit_message>
<xml_diff>
--- a/DB/DB_Schema.xlsx
+++ b/DB/DB_Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TatvaSoft\CI-Platform-Assignments\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F0FF80-9D28-4D36-830D-642C45B05EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7615415A-5550-490C-8790-1E4EBFB4C59A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{61ACD3A2-1B7E-490D-80C4-AA742D1E6BB1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="170">
   <si>
     <t>Field</t>
   </si>
@@ -432,12 +432,6 @@
     <t>mission_goal_id</t>
   </si>
   <si>
-    <t>mission_goal_objective</t>
-  </si>
-  <si>
-    <t>mission_goal_value</t>
-  </si>
-  <si>
     <t>Table mission_timesheet</t>
   </si>
   <si>
@@ -456,12 +450,6 @@
     <t>action</t>
   </si>
   <si>
-    <t>PENDING, APPROVED, DECLINED</t>
-  </si>
-  <si>
-    <t>APPROVED, PENDING, DECLINED</t>
-  </si>
-  <si>
     <t>Table banner</t>
   </si>
   <si>
@@ -532,6 +520,21 @@
   </si>
   <si>
     <t>document_path</t>
+  </si>
+  <si>
+    <t>0,1,2 - APPROVED, PENDING, DECLINED</t>
+  </si>
+  <si>
+    <t>0,1,2 - PENDING, APPROVED, DECLINED</t>
+  </si>
+  <si>
+    <t>goal_objective</t>
+  </si>
+  <si>
+    <t>goal_value</t>
+  </si>
+  <si>
+    <t>goal_achieved</t>
   </si>
 </sst>
 </file>
@@ -900,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8BA911-DC5C-494F-A61F-EE4969852268}">
-  <dimension ref="A1:H274"/>
+  <dimension ref="A1:H276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N76" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
+      <selection activeCell="E268" sqref="E268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1177,7 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D17" t="s">
         <v>23</v>
@@ -1674,7 +1677,7 @@
         <v>11</v>
       </c>
       <c r="F51" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1995,7 +1998,7 @@
         <v>11</v>
       </c>
       <c r="F75" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -2161,7 +2164,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B87" t="s">
         <v>32</v>
@@ -2169,7 +2172,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B88" t="s">
         <v>32</v>
@@ -2177,7 +2180,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B89" t="s">
         <v>21</v>
@@ -2194,7 +2197,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B90" t="s">
         <v>32</v>
@@ -2208,10 +2211,10 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B91" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D91" t="s">
         <v>23</v>
@@ -2219,10 +2222,10 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B92" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D92" t="s">
         <v>23</v>
@@ -2261,7 +2264,7 @@
         <v>61</v>
       </c>
       <c r="B95" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D95" t="s">
         <v>23</v>
@@ -2269,41 +2272,32 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="B96" t="s">
         <v>76</v>
       </c>
-      <c r="C96" t="s">
-        <v>149</v>
-      </c>
-      <c r="D96" t="s">
-        <v>10</v>
-      </c>
-      <c r="E96">
-        <v>1</v>
-      </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="B97" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C97" t="s">
-        <v>22</v>
+        <v>145</v>
       </c>
       <c r="D97" t="s">
         <v>10</v>
       </c>
-      <c r="E97" t="s">
-        <v>26</v>
+      <c r="E97">
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B98" t="s">
         <v>84</v>
@@ -2312,54 +2306,48 @@
         <v>22</v>
       </c>
       <c r="D98" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E98" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>19</v>
+      </c>
+      <c r="B99" t="s">
+        <v>84</v>
+      </c>
+      <c r="C99" t="s">
+        <v>22</v>
+      </c>
+      <c r="D99" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>20</v>
       </c>
-      <c r="B99" t="s">
-        <v>84</v>
-      </c>
-      <c r="C99" t="s">
-        <v>22</v>
-      </c>
-      <c r="D99" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="B100" t="s">
+        <v>84</v>
+      </c>
+      <c r="C100" t="s">
+        <v>22</v>
+      </c>
+      <c r="D100" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>95</v>
-      </c>
-      <c r="B102" t="s">
-        <v>9</v>
-      </c>
-      <c r="D102" t="s">
-        <v>10</v>
-      </c>
-      <c r="E102" t="s">
-        <v>11</v>
-      </c>
-      <c r="F102" t="s">
-        <v>69</v>
-      </c>
-      <c r="G102" t="s">
-        <v>13</v>
-      </c>
-      <c r="H102" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="B103" t="s">
         <v>9</v>
@@ -2370,16 +2358,19 @@
       <c r="E103" t="s">
         <v>11</v>
       </c>
+      <c r="F103" t="s">
+        <v>69</v>
+      </c>
       <c r="G103" t="s">
         <v>13</v>
       </c>
       <c r="H103" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
@@ -2394,57 +2385,60 @@
         <v>13</v>
       </c>
       <c r="H104" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="B105" t="s">
-        <v>148</v>
+        <v>9</v>
       </c>
       <c r="D105" t="s">
         <v>10</v>
+      </c>
+      <c r="E105" t="s">
+        <v>11</v>
+      </c>
+      <c r="G105" t="s">
+        <v>13</v>
+      </c>
+      <c r="H105" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B106" t="s">
-        <v>21</v>
-      </c>
-      <c r="C106" t="s">
         <v>144</v>
       </c>
       <c r="D106" t="s">
         <v>10</v>
-      </c>
-      <c r="E106" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="B107" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C107" t="s">
-        <v>22</v>
+        <v>165</v>
       </c>
       <c r="D107" t="s">
         <v>10</v>
       </c>
       <c r="E107" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B108" t="s">
         <v>84</v>
@@ -2453,54 +2447,48 @@
         <v>22</v>
       </c>
       <c r="D108" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E108" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>19</v>
+      </c>
+      <c r="B109" t="s">
+        <v>84</v>
+      </c>
+      <c r="C109" t="s">
+        <v>22</v>
+      </c>
+      <c r="D109" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>20</v>
       </c>
-      <c r="B109" t="s">
-        <v>84</v>
-      </c>
-      <c r="C109" t="s">
-        <v>22</v>
-      </c>
-      <c r="D109" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="B110" t="s">
+        <v>84</v>
+      </c>
+      <c r="C110" t="s">
+        <v>22</v>
+      </c>
+      <c r="D110" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>103</v>
-      </c>
-      <c r="B112" t="s">
-        <v>9</v>
-      </c>
-      <c r="D112" t="s">
-        <v>10</v>
-      </c>
-      <c r="E112" t="s">
-        <v>11</v>
-      </c>
-      <c r="F112" t="s">
-        <v>69</v>
-      </c>
-      <c r="G112" t="s">
-        <v>13</v>
-      </c>
-      <c r="H112" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="B113" t="s">
         <v>9</v>
@@ -2511,50 +2499,56 @@
       <c r="E113" t="s">
         <v>11</v>
       </c>
+      <c r="F113" t="s">
+        <v>69</v>
+      </c>
       <c r="G113" t="s">
         <v>13</v>
       </c>
       <c r="H113" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>163</v>
+        <v>48</v>
       </c>
       <c r="B114" t="s">
-        <v>21</v>
-      </c>
-      <c r="C114">
-        <v>128</v>
+        <v>9</v>
+      </c>
+      <c r="D114" t="s">
+        <v>10</v>
+      </c>
+      <c r="E114" t="s">
+        <v>11</v>
+      </c>
+      <c r="G114" t="s">
+        <v>13</v>
+      </c>
+      <c r="H114" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B115" t="s">
         <v>21</v>
       </c>
       <c r="C115">
-        <v>4</v>
+        <v>128</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B116" t="s">
         <v>21</v>
       </c>
       <c r="C116">
-        <v>255</v>
-      </c>
-      <c r="D116" t="s">
-        <v>23</v>
-      </c>
-      <c r="E116" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -2562,35 +2556,35 @@
         <v>161</v>
       </c>
       <c r="B117" t="s">
-        <v>56</v>
-      </c>
-      <c r="C117" t="s">
-        <v>162</v>
-      </c>
-      <c r="E117">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C117">
+        <v>255</v>
+      </c>
+      <c r="D117" t="s">
+        <v>23</v>
+      </c>
+      <c r="E117" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>18</v>
+        <v>157</v>
       </c>
       <c r="B118" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="C118" t="s">
-        <v>22</v>
-      </c>
-      <c r="D118" t="s">
-        <v>10</v>
-      </c>
-      <c r="E118" t="s">
-        <v>26</v>
+        <v>158</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B119" t="s">
         <v>84</v>
@@ -2599,54 +2593,48 @@
         <v>22</v>
       </c>
       <c r="D119" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E119" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>19</v>
+      </c>
+      <c r="B120" t="s">
+        <v>84</v>
+      </c>
+      <c r="C120" t="s">
+        <v>22</v>
+      </c>
+      <c r="D120" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>20</v>
       </c>
-      <c r="B120" t="s">
-        <v>84</v>
-      </c>
-      <c r="C120" t="s">
-        <v>22</v>
-      </c>
-      <c r="D120" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+      <c r="B121" t="s">
+        <v>84</v>
+      </c>
+      <c r="C121" t="s">
+        <v>22</v>
+      </c>
+      <c r="D121" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>97</v>
-      </c>
-      <c r="B123" t="s">
-        <v>9</v>
-      </c>
-      <c r="D123" t="s">
-        <v>10</v>
-      </c>
-      <c r="E123" t="s">
-        <v>11</v>
-      </c>
-      <c r="F123" t="s">
-        <v>69</v>
-      </c>
-      <c r="G123" t="s">
-        <v>13</v>
-      </c>
-      <c r="H123" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B124" t="s">
         <v>9</v>
@@ -2657,72 +2645,78 @@
       <c r="E124" t="s">
         <v>11</v>
       </c>
+      <c r="F124" t="s">
+        <v>69</v>
+      </c>
       <c r="G124" t="s">
         <v>13</v>
       </c>
       <c r="H124" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>166</v>
+        <v>48</v>
       </c>
       <c r="B125" t="s">
-        <v>21</v>
-      </c>
-      <c r="C125">
-        <v>128</v>
+        <v>9</v>
+      </c>
+      <c r="D125" t="s">
+        <v>10</v>
+      </c>
+      <c r="E125" t="s">
+        <v>11</v>
+      </c>
+      <c r="G125" t="s">
+        <v>13</v>
+      </c>
+      <c r="H125" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B126" t="s">
         <v>21</v>
       </c>
       <c r="C126">
-        <v>4</v>
+        <v>128</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B127" t="s">
         <v>21</v>
       </c>
       <c r="C127">
-        <v>255</v>
-      </c>
-      <c r="D127" t="s">
-        <v>23</v>
-      </c>
-      <c r="E127" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B128" t="s">
-        <v>84</v>
-      </c>
-      <c r="C128" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C128">
+        <v>255</v>
       </c>
       <c r="D128" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E128" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B129" t="s">
         <v>84</v>
@@ -2731,94 +2725,91 @@
         <v>22</v>
       </c>
       <c r="D129" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E129" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>19</v>
+      </c>
+      <c r="B130" t="s">
+        <v>84</v>
+      </c>
+      <c r="C130" t="s">
+        <v>22</v>
+      </c>
+      <c r="D130" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>20</v>
       </c>
-      <c r="B130" t="s">
-        <v>84</v>
-      </c>
-      <c r="C130" t="s">
-        <v>22</v>
-      </c>
-      <c r="D130" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="s">
+      <c r="B131" t="s">
+        <v>84</v>
+      </c>
+      <c r="C131" t="s">
+        <v>22</v>
+      </c>
+      <c r="D131" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
-      <c r="D132" s="2"/>
-      <c r="E132" s="2"/>
-      <c r="F132" s="2"/>
-      <c r="G132" s="2"/>
-      <c r="H132" s="2"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="B133" s="2"/>
       <c r="C133" s="2"/>
-      <c r="D133" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E133" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F133" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G133" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H133" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D133" s="2"/>
+      <c r="E133" s="2"/>
+      <c r="F133" s="2"/>
+      <c r="G133" s="2"/>
+      <c r="H133" s="2"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C134" s="2">
-        <v>255</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C134" s="2"/>
       <c r="D134" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F134" s="2"/>
-      <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
+      <c r="F134" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G134" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H134" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C135" s="2">
+        <v>255</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
@@ -2826,7 +2817,7 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>84</v>
@@ -2835,16 +2826,18 @@
         <v>22</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E136" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
       <c r="H136" s="2"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>84</v>
@@ -2861,19 +2854,25 @@
       <c r="H137" s="2"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" s="2"/>
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
-      <c r="D138" s="2"/>
+      <c r="A138" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E138" s="2"/>
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
       <c r="H138" s="2"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A139" s="3" t="s">
-        <v>119</v>
-      </c>
+      <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
@@ -2883,32 +2882,20 @@
       <c r="H139" s="2"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A140" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B140" s="2"/>
       <c r="C140" s="2"/>
-      <c r="D140" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E140" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G140" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H140" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
+      <c r="H140" s="2"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>9</v>
@@ -2920,17 +2907,19 @@
       <c r="E141" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F141" s="2"/>
+      <c r="F141" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="G141" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>124</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>9</v>
@@ -2947,32 +2936,34 @@
         <v>13</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>68</v>
+        <v>124</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C143" s="2"/>
       <c r="D143" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F143" s="2"/>
-      <c r="G143" s="2"/>
-      <c r="H143" s="2"/>
+      <c r="G143" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H143" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>84</v>
@@ -2981,16 +2972,18 @@
         <v>22</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E144" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
       <c r="H144" s="2"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>84</v>
@@ -3007,19 +3000,25 @@
       <c r="H145" s="2"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A146" s="2"/>
-      <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
-      <c r="D146" s="2"/>
+      <c r="A146" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2"/>
       <c r="H146" s="2"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A147" s="3" t="s">
-        <v>121</v>
-      </c>
+      <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
@@ -3029,32 +3028,20 @@
       <c r="H147" s="2"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A148" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A148" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B148" s="2"/>
       <c r="C148" s="2"/>
-      <c r="D148" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E148" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F148" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G148" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H148" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D148" s="2"/>
+      <c r="E148" s="2"/>
+      <c r="F148" s="2"/>
+      <c r="G148" s="2"/>
+      <c r="H148" s="2"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>71</v>
+        <v>122</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>9</v>
@@ -3066,17 +3053,19 @@
       <c r="E149" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F149" s="2"/>
+      <c r="F149" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="G149" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>124</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>9</v>
@@ -3093,32 +3082,34 @@
         <v>13</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C151" s="2"/>
       <c r="D151" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F151" s="2"/>
-      <c r="G151" s="2"/>
-      <c r="H151" s="2"/>
+      <c r="G151" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H151" s="2" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>84</v>
@@ -3127,16 +3118,18 @@
         <v>22</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E152" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="F152" s="2"/>
       <c r="G152" s="2"/>
       <c r="H152" s="2"/>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>84</v>
@@ -3152,37 +3145,32 @@
       <c r="G153" s="2"/>
       <c r="H153" s="2"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
+      <c r="G154" s="2"/>
+      <c r="H154" s="2"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>74</v>
-      </c>
-      <c r="B156" t="s">
-        <v>9</v>
-      </c>
-      <c r="D156" t="s">
-        <v>10</v>
-      </c>
-      <c r="E156" t="s">
-        <v>11</v>
-      </c>
-      <c r="F156" t="s">
-        <v>69</v>
-      </c>
-      <c r="G156" t="s">
-        <v>13</v>
-      </c>
-      <c r="H156" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="B157" t="s">
         <v>9</v>
@@ -3193,16 +3181,19 @@
       <c r="E157" t="s">
         <v>11</v>
       </c>
+      <c r="F157" t="s">
+        <v>69</v>
+      </c>
       <c r="G157" t="s">
         <v>13</v>
       </c>
       <c r="H157" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B158" t="s">
         <v>9</v>
@@ -3217,74 +3208,77 @@
         <v>13</v>
       </c>
       <c r="H158" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B159" t="s">
-        <v>21</v>
-      </c>
-      <c r="C159">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="D159" t="s">
         <v>10</v>
       </c>
       <c r="E159" t="s">
         <v>11</v>
+      </c>
+      <c r="G159" t="s">
+        <v>13</v>
+      </c>
+      <c r="H159" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="B160" t="s">
-        <v>84</v>
+        <v>21</v>
+      </c>
+      <c r="C160">
+        <v>80</v>
       </c>
       <c r="D160" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E160" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="B161" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="D161" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E161" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>18</v>
+        <v>147</v>
       </c>
       <c r="B162" t="s">
-        <v>84</v>
-      </c>
-      <c r="C162" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D162" t="s">
         <v>10</v>
       </c>
       <c r="E162" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B163" t="s">
         <v>84</v>
@@ -3293,54 +3287,48 @@
         <v>22</v>
       </c>
       <c r="D163" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E163" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>19</v>
+      </c>
+      <c r="B164" t="s">
+        <v>84</v>
+      </c>
+      <c r="C164" t="s">
+        <v>22</v>
+      </c>
+      <c r="D164" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>20</v>
       </c>
-      <c r="B164" t="s">
-        <v>84</v>
-      </c>
-      <c r="C164" t="s">
-        <v>22</v>
-      </c>
-      <c r="D164" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
+      <c r="B165" t="s">
+        <v>84</v>
+      </c>
+      <c r="C165" t="s">
+        <v>22</v>
+      </c>
+      <c r="D165" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>125</v>
-      </c>
-      <c r="B167" t="s">
-        <v>9</v>
-      </c>
-      <c r="D167" t="s">
-        <v>10</v>
-      </c>
-      <c r="E167" t="s">
-        <v>11</v>
-      </c>
-      <c r="F167" t="s">
-        <v>69</v>
-      </c>
-      <c r="G167" t="s">
-        <v>13</v>
-      </c>
-      <c r="H167" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="B168" t="s">
         <v>9</v>
@@ -3351,72 +3339,78 @@
       <c r="E168" t="s">
         <v>11</v>
       </c>
+      <c r="F168" t="s">
+        <v>69</v>
+      </c>
       <c r="G168" t="s">
         <v>13</v>
       </c>
       <c r="H168" t="s">
-        <v>129</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="B169" t="s">
-        <v>21</v>
-      </c>
-      <c r="C169">
-        <v>64</v>
+        <v>9</v>
+      </c>
+      <c r="D169" t="s">
+        <v>10</v>
+      </c>
+      <c r="E169" t="s">
+        <v>11</v>
+      </c>
+      <c r="G169" t="s">
+        <v>13</v>
+      </c>
+      <c r="H169" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B170" t="s">
         <v>21</v>
       </c>
       <c r="C170">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B171" t="s">
         <v>21</v>
       </c>
       <c r="C171">
-        <v>255</v>
-      </c>
-      <c r="D171" t="s">
-        <v>23</v>
-      </c>
-      <c r="E171" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>18</v>
+        <v>128</v>
       </c>
       <c r="B172" t="s">
-        <v>84</v>
-      </c>
-      <c r="C172" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C172">
+        <v>255</v>
       </c>
       <c r="D172" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E172" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B173" t="s">
         <v>84</v>
@@ -3425,54 +3419,48 @@
         <v>22</v>
       </c>
       <c r="D173" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E173" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>19</v>
+      </c>
+      <c r="B174" t="s">
+        <v>84</v>
+      </c>
+      <c r="C174" t="s">
+        <v>22</v>
+      </c>
+      <c r="D174" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>20</v>
       </c>
-      <c r="B174" t="s">
-        <v>84</v>
-      </c>
-      <c r="C174" t="s">
-        <v>22</v>
-      </c>
-      <c r="D174" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A176" s="1" t="s">
-        <v>137</v>
+      <c r="B175" t="s">
+        <v>84</v>
+      </c>
+      <c r="C175" t="s">
+        <v>22</v>
+      </c>
+      <c r="D175" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>138</v>
-      </c>
-      <c r="B177" t="s">
-        <v>9</v>
-      </c>
-      <c r="D177" t="s">
-        <v>10</v>
-      </c>
-      <c r="E177" t="s">
-        <v>11</v>
-      </c>
-      <c r="F177" t="s">
-        <v>50</v>
-      </c>
-      <c r="G177" t="s">
-        <v>13</v>
-      </c>
-      <c r="H177" t="s">
-        <v>14</v>
+      <c r="A177" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>48</v>
+        <v>136</v>
       </c>
       <c r="B178" t="s">
         <v>9</v>
@@ -3483,16 +3471,19 @@
       <c r="E178" t="s">
         <v>11</v>
       </c>
+      <c r="F178" t="s">
+        <v>50</v>
+      </c>
       <c r="G178" t="s">
         <v>13</v>
       </c>
       <c r="H178" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B179" t="s">
         <v>9</v>
@@ -3507,51 +3498,57 @@
         <v>13</v>
       </c>
       <c r="H179" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="B180" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="D180" t="s">
         <v>10</v>
+      </c>
+      <c r="E180" t="s">
+        <v>11</v>
+      </c>
+      <c r="G180" t="s">
+        <v>13</v>
+      </c>
+      <c r="H180" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="B181" t="s">
-        <v>139</v>
+        <v>58</v>
       </c>
       <c r="D181" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B182" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
       <c r="D182" t="s">
         <v>23</v>
-      </c>
-      <c r="E182" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B183" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D183" t="s">
         <v>23</v>
@@ -3562,41 +3559,38 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="B184" t="s">
-        <v>21</v>
-      </c>
-      <c r="C184" t="s">
-        <v>143</v>
+        <v>30</v>
       </c>
       <c r="D184" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E184" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B185" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C185" t="s">
-        <v>22</v>
+        <v>166</v>
       </c>
       <c r="D185" t="s">
         <v>10</v>
       </c>
       <c r="E185" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B186" t="s">
         <v>84</v>
@@ -3605,54 +3599,48 @@
         <v>22</v>
       </c>
       <c r="D186" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E186" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>19</v>
+      </c>
+      <c r="B187" t="s">
+        <v>84</v>
+      </c>
+      <c r="C187" t="s">
+        <v>22</v>
+      </c>
+      <c r="D187" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>20</v>
       </c>
-      <c r="B187" t="s">
-        <v>84</v>
-      </c>
-      <c r="C187" t="s">
-        <v>22</v>
-      </c>
-      <c r="D187" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A189" s="1" t="s">
+      <c r="B188" t="s">
+        <v>84</v>
+      </c>
+      <c r="C188" t="s">
+        <v>22</v>
+      </c>
+      <c r="D188" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>134</v>
-      </c>
-      <c r="B190" t="s">
-        <v>9</v>
-      </c>
-      <c r="D190" t="s">
-        <v>10</v>
-      </c>
-      <c r="E190" t="s">
-        <v>11</v>
-      </c>
-      <c r="F190" t="s">
-        <v>50</v>
-      </c>
-      <c r="G190" t="s">
-        <v>13</v>
-      </c>
-      <c r="H190" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>48</v>
+        <v>134</v>
       </c>
       <c r="B191" t="s">
         <v>9</v>
@@ -3663,157 +3651,157 @@
       <c r="E191" t="s">
         <v>11</v>
       </c>
+      <c r="F191" t="s">
+        <v>50</v>
+      </c>
       <c r="G191" t="s">
         <v>13</v>
       </c>
       <c r="H191" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>135</v>
+        <v>48</v>
       </c>
       <c r="B192" t="s">
-        <v>21</v>
-      </c>
-      <c r="C192">
-        <v>255</v>
+        <v>9</v>
       </c>
       <c r="D192" t="s">
         <v>10</v>
       </c>
       <c r="E192" t="s">
         <v>11</v>
+      </c>
+      <c r="G192" t="s">
+        <v>13</v>
+      </c>
+      <c r="H192" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
       <c r="B193" t="s">
-        <v>30</v>
+        <v>21</v>
+      </c>
+      <c r="C193">
+        <v>255</v>
       </c>
       <c r="D193" t="s">
         <v>10</v>
+      </c>
+      <c r="E193" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>18</v>
+        <v>168</v>
       </c>
       <c r="B194" t="s">
-        <v>84</v>
-      </c>
-      <c r="C194" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D194" t="s">
         <v>10</v>
-      </c>
-      <c r="E194" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>19</v>
+        <v>169</v>
       </c>
       <c r="B195" t="s">
-        <v>84</v>
-      </c>
-      <c r="C195" t="s">
-        <v>22</v>
-      </c>
-      <c r="D195" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="E195">
+        <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
+        <v>18</v>
+      </c>
+      <c r="B196" t="s">
+        <v>84</v>
+      </c>
+      <c r="C196" t="s">
+        <v>22</v>
+      </c>
+      <c r="D196" t="s">
+        <v>10</v>
+      </c>
+      <c r="E196" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>19</v>
+      </c>
+      <c r="B197" t="s">
+        <v>84</v>
+      </c>
+      <c r="C197" t="s">
+        <v>22</v>
+      </c>
+      <c r="D197" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
         <v>20</v>
       </c>
-      <c r="B196" t="s">
-        <v>84</v>
-      </c>
-      <c r="C196" t="s">
-        <v>22</v>
-      </c>
-      <c r="D196" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A198" s="1" t="s">
+      <c r="B198" t="s">
+        <v>84</v>
+      </c>
+      <c r="C198" t="s">
+        <v>22</v>
+      </c>
+      <c r="D198" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>78</v>
-      </c>
-      <c r="B199" t="s">
-        <v>9</v>
-      </c>
-      <c r="D199" t="s">
-        <v>10</v>
-      </c>
-      <c r="E199" t="s">
-        <v>11</v>
-      </c>
-      <c r="F199" t="s">
-        <v>69</v>
-      </c>
-      <c r="G199" t="s">
-        <v>13</v>
-      </c>
-      <c r="H199" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>158</v>
-      </c>
-      <c r="B200" t="s">
-        <v>21</v>
-      </c>
-      <c r="C200">
-        <v>30</v>
-      </c>
-      <c r="D200" t="s">
-        <v>10</v>
-      </c>
-      <c r="E200" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="B201" t="s">
-        <v>21</v>
-      </c>
-      <c r="C201">
-        <v>128</v>
+        <v>9</v>
       </c>
       <c r="D201" t="s">
         <v>10</v>
       </c>
       <c r="E201" t="s">
         <v>11</v>
+      </c>
+      <c r="F201" t="s">
+        <v>69</v>
+      </c>
+      <c r="G201" t="s">
+        <v>13</v>
+      </c>
+      <c r="H201" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B202" t="s">
         <v>21</v>
       </c>
       <c r="C202">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="D202" t="s">
         <v>10</v>
@@ -3824,10 +3812,13 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>160</v>
+        <v>17</v>
       </c>
       <c r="B203" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="C203">
+        <v>128</v>
       </c>
       <c r="D203" t="s">
         <v>10</v>
@@ -3838,226 +3829,226 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>43</v>
+        <v>155</v>
       </c>
       <c r="B204" t="s">
-        <v>56</v>
-      </c>
-      <c r="C204" t="s">
-        <v>44</v>
+        <v>21</v>
+      </c>
+      <c r="C204">
+        <v>200</v>
       </c>
       <c r="D204" t="s">
         <v>10</v>
       </c>
-      <c r="E204">
-        <v>0</v>
+      <c r="E204" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
+        <v>156</v>
+      </c>
+      <c r="B205" t="s">
+        <v>32</v>
+      </c>
+      <c r="D205" t="s">
+        <v>10</v>
+      </c>
+      <c r="E205" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>43</v>
+      </c>
+      <c r="B206" t="s">
+        <v>56</v>
+      </c>
+      <c r="C206" t="s">
+        <v>44</v>
+      </c>
+      <c r="D206" t="s">
+        <v>10</v>
+      </c>
+      <c r="E206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
         <v>18</v>
       </c>
-      <c r="B205" t="s">
-        <v>84</v>
-      </c>
-      <c r="C205" t="s">
-        <v>22</v>
-      </c>
-      <c r="D205" t="s">
-        <v>10</v>
-      </c>
-      <c r="E205" t="s">
+      <c r="B207" t="s">
+        <v>84</v>
+      </c>
+      <c r="C207" t="s">
+        <v>22</v>
+      </c>
+      <c r="D207" t="s">
+        <v>10</v>
+      </c>
+      <c r="E207" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A207" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>79</v>
-      </c>
-      <c r="B208" t="s">
-        <v>30</v>
-      </c>
-      <c r="D208" t="s">
-        <v>10</v>
-      </c>
-      <c r="E208" t="s">
-        <v>11</v>
-      </c>
-      <c r="F208" t="s">
-        <v>69</v>
-      </c>
-      <c r="G208" t="s">
-        <v>13</v>
-      </c>
-      <c r="H208" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>87</v>
-      </c>
-      <c r="B209" t="s">
-        <v>21</v>
-      </c>
-      <c r="C209" t="s">
-        <v>146</v>
-      </c>
-      <c r="D209" t="s">
-        <v>10</v>
-      </c>
-      <c r="E209" t="s">
-        <v>11</v>
+      <c r="A209" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>157</v>
+        <v>79</v>
       </c>
       <c r="B210" t="s">
         <v>30</v>
       </c>
-      <c r="E210">
-        <v>0</v>
+      <c r="D210" t="s">
+        <v>10</v>
+      </c>
+      <c r="E210" t="s">
+        <v>11</v>
+      </c>
+      <c r="F210" t="s">
+        <v>69</v>
+      </c>
+      <c r="G210" t="s">
+        <v>13</v>
+      </c>
+      <c r="H210" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="B211" t="s">
         <v>21</v>
       </c>
-      <c r="C211">
-        <v>300</v>
+      <c r="C211" t="s">
+        <v>142</v>
       </c>
       <c r="D211" t="s">
         <v>10</v>
       </c>
       <c r="E211" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B212" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E212">
+        <v>0</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B213" t="s">
-        <v>84</v>
-      </c>
-      <c r="C213" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C213">
+        <v>300</v>
       </c>
       <c r="D213" t="s">
         <v>10</v>
       </c>
       <c r="E213" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="B214" t="s">
-        <v>84</v>
-      </c>
-      <c r="C214" t="s">
-        <v>22</v>
-      </c>
-      <c r="D214" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
+        <v>18</v>
+      </c>
+      <c r="B215" t="s">
+        <v>84</v>
+      </c>
+      <c r="C215" t="s">
+        <v>22</v>
+      </c>
+      <c r="D215" t="s">
+        <v>10</v>
+      </c>
+      <c r="E215" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>19</v>
+      </c>
+      <c r="B216" t="s">
+        <v>84</v>
+      </c>
+      <c r="C216" t="s">
+        <v>22</v>
+      </c>
+      <c r="D216" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>20</v>
       </c>
-      <c r="B215" t="s">
-        <v>84</v>
-      </c>
-      <c r="C215" t="s">
-        <v>22</v>
-      </c>
-      <c r="D215" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A217" s="1" t="s">
+      <c r="B217" t="s">
+        <v>84</v>
+      </c>
+      <c r="C217" t="s">
+        <v>22</v>
+      </c>
+      <c r="D217" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>81</v>
-      </c>
-      <c r="B218" t="s">
-        <v>45</v>
-      </c>
-      <c r="D218" t="s">
-        <v>10</v>
-      </c>
-      <c r="E218" t="s">
-        <v>11</v>
-      </c>
-      <c r="F218" t="s">
-        <v>69</v>
-      </c>
-      <c r="G218" t="s">
-        <v>82</v>
-      </c>
-      <c r="H218" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>42</v>
-      </c>
-      <c r="B219" t="s">
-        <v>21</v>
-      </c>
-      <c r="C219">
-        <v>255</v>
-      </c>
-      <c r="D219" t="s">
-        <v>10</v>
-      </c>
-      <c r="E219" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>151</v>
+        <v>81</v>
       </c>
       <c r="B220" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D220" t="s">
         <v>10</v>
       </c>
       <c r="E220" t="s">
         <v>11</v>
+      </c>
+      <c r="F220" t="s">
+        <v>69</v>
+      </c>
+      <c r="G220" t="s">
+        <v>82</v>
+      </c>
+      <c r="H220" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>156</v>
+        <v>42</v>
       </c>
       <c r="B221" t="s">
         <v>21</v>
@@ -4066,125 +4057,113 @@
         <v>255</v>
       </c>
       <c r="D221" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E221" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="B222" t="s">
-        <v>56</v>
-      </c>
-      <c r="C222" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D222" t="s">
         <v>10</v>
       </c>
-      <c r="E222">
-        <v>1</v>
+      <c r="E222" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>18</v>
+        <v>152</v>
       </c>
       <c r="B223" t="s">
-        <v>84</v>
-      </c>
-      <c r="C223" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C223">
+        <v>255</v>
       </c>
       <c r="D223" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E223" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="B224" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="C224" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D224" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E224">
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
+        <v>18</v>
+      </c>
+      <c r="B225" t="s">
+        <v>84</v>
+      </c>
+      <c r="C225" t="s">
+        <v>22</v>
+      </c>
+      <c r="D225" t="s">
+        <v>10</v>
+      </c>
+      <c r="E225" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>19</v>
+      </c>
+      <c r="B226" t="s">
+        <v>84</v>
+      </c>
+      <c r="C226" t="s">
+        <v>22</v>
+      </c>
+      <c r="D226" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
         <v>20</v>
       </c>
-      <c r="B225" t="s">
-        <v>84</v>
-      </c>
-      <c r="C225" t="s">
-        <v>22</v>
-      </c>
-      <c r="D225" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A227" s="1" t="s">
+      <c r="B227" t="s">
+        <v>84</v>
+      </c>
+      <c r="C227" t="s">
+        <v>22</v>
+      </c>
+      <c r="D227" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
-        <v>89</v>
-      </c>
-      <c r="B228" t="s">
-        <v>9</v>
-      </c>
-      <c r="D228" t="s">
-        <v>10</v>
-      </c>
-      <c r="E228" t="s">
-        <v>11</v>
-      </c>
-      <c r="F228" t="s">
-        <v>69</v>
-      </c>
-      <c r="G228" t="s">
-        <v>13</v>
-      </c>
-      <c r="H228" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>48</v>
-      </c>
-      <c r="B229" t="s">
-        <v>9</v>
-      </c>
-      <c r="D229" t="s">
-        <v>10</v>
-      </c>
-      <c r="E229" t="s">
-        <v>11</v>
-      </c>
-      <c r="G229" t="s">
-        <v>13</v>
-      </c>
-      <c r="H229" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="B230" t="s">
         <v>9</v>
@@ -4195,126 +4174,126 @@
       <c r="E230" t="s">
         <v>11</v>
       </c>
+      <c r="F230" t="s">
+        <v>69</v>
+      </c>
       <c r="G230" t="s">
         <v>13</v>
       </c>
       <c r="H230" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="B231" t="s">
-        <v>21</v>
-      </c>
-      <c r="C231" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="D231" t="s">
         <v>10</v>
       </c>
       <c r="E231" t="s">
-        <v>92</v>
+        <v>11</v>
+      </c>
+      <c r="G231" t="s">
+        <v>13</v>
+      </c>
+      <c r="H231" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B232" t="s">
-        <v>84</v>
-      </c>
-      <c r="C232" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D232" t="s">
         <v>10</v>
       </c>
       <c r="E232" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="G232" t="s">
+        <v>13</v>
+      </c>
+      <c r="H232" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="B233" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C233" t="s">
-        <v>22</v>
+        <v>166</v>
       </c>
       <c r="D233" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E233" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
+        <v>18</v>
+      </c>
+      <c r="B234" t="s">
+        <v>84</v>
+      </c>
+      <c r="C234" t="s">
+        <v>22</v>
+      </c>
+      <c r="D234" t="s">
+        <v>10</v>
+      </c>
+      <c r="E234" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>19</v>
+      </c>
+      <c r="B235" t="s">
+        <v>84</v>
+      </c>
+      <c r="C235" t="s">
+        <v>22</v>
+      </c>
+      <c r="D235" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
         <v>20</v>
       </c>
-      <c r="B234" t="s">
-        <v>84</v>
-      </c>
-      <c r="C234" t="s">
-        <v>22</v>
-      </c>
-      <c r="D234" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A236" s="1" t="s">
+      <c r="B236" t="s">
+        <v>84</v>
+      </c>
+      <c r="C236" t="s">
+        <v>22</v>
+      </c>
+      <c r="D236" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>94</v>
-      </c>
-      <c r="B237" t="s">
-        <v>9</v>
-      </c>
-      <c r="D237" t="s">
-        <v>10</v>
-      </c>
-      <c r="E237" t="s">
-        <v>11</v>
-      </c>
-      <c r="F237" t="s">
-        <v>69</v>
-      </c>
-      <c r="G237" t="s">
-        <v>13</v>
-      </c>
-      <c r="H237" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>48</v>
-      </c>
-      <c r="B238" t="s">
-        <v>9</v>
-      </c>
-      <c r="D238" t="s">
-        <v>10</v>
-      </c>
-      <c r="E238" t="s">
-        <v>11</v>
-      </c>
-      <c r="G238" t="s">
-        <v>13</v>
-      </c>
-      <c r="H238" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="B239" t="s">
         <v>9</v>
@@ -4325,109 +4304,109 @@
       <c r="E239" t="s">
         <v>11</v>
       </c>
+      <c r="F239" t="s">
+        <v>69</v>
+      </c>
       <c r="G239" t="s">
         <v>13</v>
       </c>
       <c r="H239" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B240" t="s">
-        <v>84</v>
-      </c>
-      <c r="C240" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D240" t="s">
         <v>10</v>
       </c>
       <c r="E240" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="G240" t="s">
+        <v>13</v>
+      </c>
+      <c r="H240" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B241" t="s">
-        <v>84</v>
-      </c>
-      <c r="C241" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D241" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E241" t="s">
+        <v>11</v>
+      </c>
+      <c r="G241" t="s">
+        <v>13</v>
+      </c>
+      <c r="H241" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
+        <v>18</v>
+      </c>
+      <c r="B242" t="s">
+        <v>84</v>
+      </c>
+      <c r="C242" t="s">
+        <v>22</v>
+      </c>
+      <c r="D242" t="s">
+        <v>10</v>
+      </c>
+      <c r="E242" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>19</v>
+      </c>
+      <c r="B243" t="s">
+        <v>84</v>
+      </c>
+      <c r="C243" t="s">
+        <v>22</v>
+      </c>
+      <c r="D243" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
         <v>20</v>
       </c>
-      <c r="B242" t="s">
-        <v>84</v>
-      </c>
-      <c r="C242" t="s">
-        <v>22</v>
-      </c>
-      <c r="D242" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
+      <c r="B244" t="s">
+        <v>84</v>
+      </c>
+      <c r="C244" t="s">
+        <v>22</v>
+      </c>
+      <c r="D244" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>99</v>
-      </c>
-      <c r="B245" t="s">
-        <v>9</v>
-      </c>
-      <c r="D245" t="s">
-        <v>10</v>
-      </c>
-      <c r="E245" t="s">
-        <v>11</v>
-      </c>
-      <c r="F245" t="s">
-        <v>69</v>
-      </c>
-      <c r="G245" t="s">
-        <v>13</v>
-      </c>
-      <c r="H245" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
-        <v>48</v>
-      </c>
-      <c r="B246" t="s">
-        <v>9</v>
-      </c>
-      <c r="D246" t="s">
-        <v>10</v>
-      </c>
-      <c r="E246" t="s">
-        <v>11</v>
-      </c>
-      <c r="G246" t="s">
-        <v>13</v>
-      </c>
-      <c r="H246" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B247" t="s">
         <v>9</v>
@@ -4438,16 +4417,19 @@
       <c r="E247" t="s">
         <v>11</v>
       </c>
+      <c r="F247" t="s">
+        <v>69</v>
+      </c>
       <c r="G247" t="s">
         <v>13</v>
       </c>
       <c r="H247" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="B248" t="s">
         <v>9</v>
@@ -4462,105 +4444,102 @@
         <v>13</v>
       </c>
       <c r="H248" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="B249" t="s">
-        <v>84</v>
-      </c>
-      <c r="C249" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D249" t="s">
         <v>10</v>
       </c>
       <c r="E249" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="G249" t="s">
+        <v>13</v>
+      </c>
+      <c r="H249" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="B250" t="s">
-        <v>84</v>
-      </c>
-      <c r="C250" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D250" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E250" t="s">
+        <v>11</v>
+      </c>
+      <c r="G250" t="s">
+        <v>13</v>
+      </c>
+      <c r="H250" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
+        <v>18</v>
+      </c>
+      <c r="B251" t="s">
+        <v>84</v>
+      </c>
+      <c r="C251" t="s">
+        <v>22</v>
+      </c>
+      <c r="D251" t="s">
+        <v>10</v>
+      </c>
+      <c r="E251" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>19</v>
+      </c>
+      <c r="B252" t="s">
+        <v>84</v>
+      </c>
+      <c r="C252" t="s">
+        <v>22</v>
+      </c>
+      <c r="D252" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
         <v>20</v>
       </c>
-      <c r="B251" t="s">
-        <v>84</v>
-      </c>
-      <c r="C251" t="s">
-        <v>22</v>
-      </c>
-      <c r="D251" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A253" s="1" t="s">
+      <c r="B253" t="s">
+        <v>84</v>
+      </c>
+      <c r="C253" t="s">
+        <v>22</v>
+      </c>
+      <c r="D253" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>132</v>
-      </c>
-      <c r="B254" t="s">
-        <v>9</v>
-      </c>
-      <c r="D254" t="s">
-        <v>10</v>
-      </c>
-      <c r="E254" t="s">
-        <v>11</v>
-      </c>
-      <c r="F254" t="s">
-        <v>69</v>
-      </c>
-      <c r="G254" t="s">
-        <v>13</v>
-      </c>
-      <c r="H254" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
-        <v>74</v>
-      </c>
-      <c r="B255" t="s">
-        <v>9</v>
-      </c>
-      <c r="D255" t="s">
-        <v>10</v>
-      </c>
-      <c r="E255" t="s">
-        <v>11</v>
-      </c>
-      <c r="G255" t="s">
-        <v>13</v>
-      </c>
-      <c r="H255" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="B256" t="s">
         <v>9</v>
@@ -4571,16 +4550,19 @@
       <c r="E256" t="s">
         <v>11</v>
       </c>
+      <c r="F256" t="s">
+        <v>69</v>
+      </c>
       <c r="G256" t="s">
         <v>13</v>
       </c>
       <c r="H256" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="B257" t="s">
         <v>9</v>
@@ -4595,105 +4577,102 @@
         <v>13</v>
       </c>
       <c r="H257" t="s">
-        <v>90</v>
+        <v>129</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="B258" t="s">
-        <v>84</v>
-      </c>
-      <c r="C258" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D258" t="s">
         <v>10</v>
       </c>
       <c r="E258" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="G258" t="s">
+        <v>13</v>
+      </c>
+      <c r="H258" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="B259" t="s">
-        <v>84</v>
-      </c>
-      <c r="C259" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D259" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E259" t="s">
+        <v>11</v>
+      </c>
+      <c r="G259" t="s">
+        <v>13</v>
+      </c>
+      <c r="H259" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
+        <v>18</v>
+      </c>
+      <c r="B260" t="s">
+        <v>84</v>
+      </c>
+      <c r="C260" t="s">
+        <v>22</v>
+      </c>
+      <c r="D260" t="s">
+        <v>10</v>
+      </c>
+      <c r="E260" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>19</v>
+      </c>
+      <c r="B261" t="s">
+        <v>84</v>
+      </c>
+      <c r="C261" t="s">
+        <v>22</v>
+      </c>
+      <c r="D261" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
         <v>20</v>
       </c>
-      <c r="B260" t="s">
-        <v>84</v>
-      </c>
-      <c r="C260" t="s">
-        <v>22</v>
-      </c>
-      <c r="D260" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A262" s="1" t="s">
+      <c r="B262" t="s">
+        <v>84</v>
+      </c>
+      <c r="C262" t="s">
+        <v>22</v>
+      </c>
+      <c r="D262" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
-        <v>105</v>
-      </c>
-      <c r="B263" t="s">
-        <v>9</v>
-      </c>
-      <c r="D263" t="s">
-        <v>10</v>
-      </c>
-      <c r="E263" t="s">
-        <v>11</v>
-      </c>
-      <c r="F263" t="s">
-        <v>69</v>
-      </c>
-      <c r="G263" t="s">
-        <v>13</v>
-      </c>
-      <c r="H263" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A264" t="s">
-        <v>48</v>
-      </c>
-      <c r="B264" t="s">
-        <v>9</v>
-      </c>
-      <c r="D264" t="s">
-        <v>10</v>
-      </c>
-      <c r="E264" t="s">
-        <v>11</v>
-      </c>
-      <c r="G264" t="s">
-        <v>13</v>
-      </c>
-      <c r="H264" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="B265" t="s">
         <v>9</v>
@@ -4704,125 +4683,168 @@
       <c r="E265" t="s">
         <v>11</v>
       </c>
+      <c r="F265" t="s">
+        <v>69</v>
+      </c>
       <c r="G265" t="s">
         <v>13</v>
       </c>
       <c r="H265" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="B266" t="s">
-        <v>76</v>
-      </c>
-      <c r="C266" t="s">
-        <v>107</v>
+        <v>9</v>
       </c>
       <c r="D266" t="s">
         <v>10</v>
       </c>
       <c r="E266" t="s">
         <v>11</v>
+      </c>
+      <c r="G266" t="s">
+        <v>13</v>
+      </c>
+      <c r="H266" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B267" t="s">
-        <v>84</v>
-      </c>
-      <c r="C267" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D267" t="s">
         <v>10</v>
       </c>
       <c r="E267" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="G267" t="s">
+        <v>13</v>
+      </c>
+      <c r="H267" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="B268" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C268" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="D268" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E268" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
+        <v>18</v>
+      </c>
+      <c r="B269" t="s">
+        <v>84</v>
+      </c>
+      <c r="C269" t="s">
+        <v>22</v>
+      </c>
+      <c r="D269" t="s">
+        <v>10</v>
+      </c>
+      <c r="E269" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>19</v>
+      </c>
+      <c r="B270" t="s">
+        <v>84</v>
+      </c>
+      <c r="C270" t="s">
+        <v>22</v>
+      </c>
+      <c r="D270" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
         <v>20</v>
       </c>
-      <c r="B269" t="s">
-        <v>84</v>
-      </c>
-      <c r="C269" t="s">
-        <v>22</v>
-      </c>
-      <c r="D269" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A271" s="1" t="s">
+      <c r="B271" t="s">
+        <v>84</v>
+      </c>
+      <c r="C271" t="s">
+        <v>22</v>
+      </c>
+      <c r="D271" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A272" t="s">
-        <v>17</v>
-      </c>
-      <c r="B272" t="s">
-        <v>21</v>
-      </c>
-      <c r="C272">
-        <v>128</v>
-      </c>
-      <c r="D272" t="s">
-        <v>10</v>
-      </c>
-      <c r="E272" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
-        <v>110</v>
-      </c>
-      <c r="B273" t="s">
-        <v>21</v>
-      </c>
-      <c r="C273">
-        <v>255</v>
-      </c>
-      <c r="D273" t="s">
-        <v>10</v>
-      </c>
-      <c r="E273" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
+        <v>17</v>
+      </c>
+      <c r="B274" t="s">
+        <v>21</v>
+      </c>
+      <c r="C274">
+        <v>128</v>
+      </c>
+      <c r="D274" t="s">
+        <v>10</v>
+      </c>
+      <c r="E274" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>110</v>
+      </c>
+      <c r="B275" t="s">
+        <v>21</v>
+      </c>
+      <c r="C275">
+        <v>255</v>
+      </c>
+      <c r="D275" t="s">
+        <v>10</v>
+      </c>
+      <c r="E275" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
         <v>18</v>
       </c>
-      <c r="B274" t="s">
-        <v>84</v>
-      </c>
-      <c r="D274" t="s">
-        <v>10</v>
-      </c>
-      <c r="E274" t="s">
+      <c r="B276" t="s">
+        <v>84</v>
+      </c>
+      <c r="D276" t="s">
+        <v>10</v>
+      </c>
+      <c r="E276" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on share story page
</commit_message>
<xml_diff>
--- a/DB/DB_Schema.xlsx
+++ b/DB/DB_Schema.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="172">
   <si>
     <t xml:space="preserve">Table admin</t>
   </si>
@@ -310,7 +310,7 @@
     <t xml:space="preserve">approval_status</t>
   </si>
   <si>
-    <t xml:space="preserve">0,1,2 - APPROVED, PENDING, DECLINED</t>
+    <t xml:space="preserve">0,1,2 – PENDING, APPROVED, DECLINED</t>
   </si>
   <si>
     <t xml:space="preserve">PENDING</t>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t xml:space="preserve">published_at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,1,2,3 – pending, approved, declined, draft</t>
   </si>
   <si>
     <t xml:space="preserve">Table story_media</t>
@@ -716,10 +719,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H277"/>
+  <dimension ref="A1:H279"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A218" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E233" activeCellId="0" sqref="233:233"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A144" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C163" activeCellId="0" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -729,7 +732,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="35.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.67"/>
@@ -3091,32 +3094,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D163" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E163" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C164" s="0" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D164" s="0" t="s">
         <v>18</v>
@@ -3124,201 +3118,189 @@
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C165" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D165" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E165" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B166" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C166" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D166" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B165" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C165" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D165" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="0" t="s">
+      <c r="B167" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C167" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D167" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B168" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D168" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E168" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F168" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G168" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H168" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B169" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D169" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E169" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G169" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H169" s="0" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C170" s="0" t="n">
-        <v>64</v>
+        <v>31</v>
+      </c>
+      <c r="D170" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E170" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F170" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G170" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H170" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C171" s="0" t="n">
-        <v>4</v>
+        <v>31</v>
+      </c>
+      <c r="D171" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E171" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G171" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H171" s="0" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B172" s="0" t="s">
         <v>17</v>
       </c>
       <c r="C172" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="D172" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E172" s="0" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>23</v>
+        <v>127</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C173" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D173" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E173" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="C173" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>27</v>
+        <v>128</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C174" s="0" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="C174" s="0" t="n">
+        <v>255</v>
       </c>
       <c r="D174" s="0" t="s">
         <v>18</v>
+      </c>
+      <c r="E174" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C175" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D175" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E175" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B176" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C176" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D176" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B175" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C175" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D175" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="0" t="s">
+      <c r="B177" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C177" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D177" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B178" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D178" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E178" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F178" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G178" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H178" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B179" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D179" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E179" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G179" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H179" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="B180" s="0" t="s">
         <v>31</v>
@@ -3329,171 +3311,171 @@
       <c r="E180" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="F180" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="G180" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H180" s="0" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>130</v>
+        <v>68</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>131</v>
+        <v>31</v>
       </c>
       <c r="D181" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="E181" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G181" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H181" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>132</v>
+        <v>30</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>133</v>
+        <v>31</v>
       </c>
       <c r="D182" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E182" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G182" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H182" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="D183" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E183" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="D184" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="E184" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C185" s="0" t="s">
-        <v>136</v>
+        <v>37</v>
       </c>
       <c r="D185" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E185" s="0" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C186" s="0" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D186" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E186" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C187" s="0" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="D187" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E187" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B188" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C188" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D188" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E188" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B189" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C189" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D189" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B188" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C188" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D188" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="0" t="s">
+      <c r="B190" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C190" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D190" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B191" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D191" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E191" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F191" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G191" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H191" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B192" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D192" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E192" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G192" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H192" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3501,145 +3483,154 @@
         <v>139</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C193" s="0" t="n">
-        <v>255</v>
+        <v>31</v>
       </c>
       <c r="D193" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E193" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="F193" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G193" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H193" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D194" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="E194" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G194" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H194" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E195" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="C195" s="0" t="n">
+        <v>255</v>
+      </c>
+      <c r="D195" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E195" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C196" s="0" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D196" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="E196" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C197" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D197" s="0" t="s">
-        <v>18</v>
+        <v>42</v>
+      </c>
+      <c r="E197" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B198" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C198" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D198" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E198" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B199" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C199" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D199" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B198" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C198" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D198" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="0" t="s">
+      <c r="B200" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C200" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D200" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B201" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D201" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E201" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F201" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G201" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H201" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B202" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C202" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="D202" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E202" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>21</v>
+        <v>144</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C203" s="0" t="n">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="D203" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E203" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="F203" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G203" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H203" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3650,7 +3641,7 @@
         <v>17</v>
       </c>
       <c r="C204" s="0" t="n">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="D204" s="0" t="s">
         <v>11</v>
@@ -3661,10 +3652,13 @@
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>146</v>
+        <v>21</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
+      </c>
+      <c r="C205" s="0" t="n">
+        <v>128</v>
       </c>
       <c r="D205" s="0" t="s">
         <v>11</v>
@@ -3675,226 +3669,226 @@
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>50</v>
+        <v>146</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C206" s="0" t="s">
-        <v>52</v>
+        <v>17</v>
+      </c>
+      <c r="C206" s="0" t="n">
+        <v>200</v>
       </c>
       <c r="D206" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E206" s="0" t="n">
-        <v>0</v>
+      <c r="E206" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D207" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E207" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B208" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C208" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D208" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E208" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B207" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C207" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D207" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E207" s="0" t="s">
+      <c r="B209" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C209" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D209" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E209" s="0" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="0" t="s">
+    <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="B210" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D210" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E210" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F210" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G210" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H210" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B211" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C211" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D211" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E211" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B212" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E212" s="0" t="n">
-        <v>0</v>
+      <c r="D212" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E212" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F212" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G212" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H212" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>49</v>
+        <v>150</v>
       </c>
       <c r="B213" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C213" s="0" t="n">
-        <v>300</v>
+      <c r="C213" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="D213" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E213" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>79</v>
+        <v>151</v>
       </c>
       <c r="B214" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="E214" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C215" s="0" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="C215" s="0" t="n">
+        <v>300</v>
       </c>
       <c r="D215" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E215" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C216" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D216" s="0" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B217" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C217" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D217" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E217" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B218" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C218" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D218" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B217" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C217" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D217" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="0" t="s">
+      <c r="B219" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C219" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D219" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B220" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D220" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E220" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F220" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G220" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="H220" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B221" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C221" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="D221" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E221" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>79</v>
+        <v>153</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D222" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E222" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="F222" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G222" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="H222" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>154</v>
+        <v>49</v>
       </c>
       <c r="B223" s="0" t="s">
         <v>17</v>
@@ -3903,125 +3897,113 @@
         <v>255</v>
       </c>
       <c r="D223" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E223" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C224" s="0" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D224" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E224" s="0" t="n">
-        <v>1</v>
+      <c r="E224" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>23</v>
+        <v>155</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C225" s="0" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="C225" s="0" t="n">
+        <v>255</v>
       </c>
       <c r="D225" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E225" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D226" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E226" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B227" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C227" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D227" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E227" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B228" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C228" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D228" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B227" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C227" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D227" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="0" t="s">
+      <c r="B229" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C229" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D229" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="B230" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D230" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E230" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F230" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G230" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H230" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B231" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D231" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E231" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G231" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H231" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="B232" s="0" t="s">
         <v>31</v>
@@ -4032,137 +4014,137 @@
       <c r="E232" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="F232" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="G232" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H232" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>157</v>
+        <v>68</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D233" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="E233" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G233" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H233" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C234" s="0" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="D234" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E234" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="G234" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H234" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>23</v>
+        <v>158</v>
       </c>
       <c r="B235" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C235" s="0" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D235" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="E235" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="B236" s="0" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C236" s="0" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="D236" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E236" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B237" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C237" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D237" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E237" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B238" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C238" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D238" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B237" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C237" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D237" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="0" t="s">
+      <c r="B239" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C239" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D239" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B240" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D240" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E240" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F240" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G240" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H240" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B241" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D241" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E241" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G241" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H241" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>30</v>
+        <v>160</v>
       </c>
       <c r="B242" s="0" t="s">
         <v>31</v>
@@ -4173,104 +4155,104 @@
       <c r="E242" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="F242" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="G242" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H242" s="0" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="B243" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C243" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D243" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E243" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="G243" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H243" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B244" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C244" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D244" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E244" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G244" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H244" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B245" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C245" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D245" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E245" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B246" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C246" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D246" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B245" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C245" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D245" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="0" t="s">
+      <c r="B247" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C247" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D247" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B248" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D248" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E248" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F248" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G248" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H248" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B249" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D249" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E249" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G249" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H249" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4286,16 +4268,19 @@
       <c r="E250" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="F250" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="G250" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H250" s="0" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>163</v>
+        <v>68</v>
       </c>
       <c r="B251" s="0" t="s">
         <v>31</v>
@@ -4310,105 +4295,102 @@
         <v>14</v>
       </c>
       <c r="H251" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>23</v>
+        <v>163</v>
       </c>
       <c r="B252" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C252" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D252" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E252" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="G252" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H252" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>27</v>
+        <v>164</v>
       </c>
       <c r="B253" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C253" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D253" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E253" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G253" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H253" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B254" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C254" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D254" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E254" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B255" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C255" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D255" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B254" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C254" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D254" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="0" t="s">
+      <c r="B256" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C256" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D256" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="B257" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D257" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E257" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F257" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G257" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H257" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B258" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D258" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E258" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G258" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H258" s="0" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B259" s="0" t="s">
         <v>31</v>
@@ -4419,16 +4401,19 @@
       <c r="E259" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="F259" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="G259" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H259" s="0" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
-        <v>163</v>
+        <v>118</v>
       </c>
       <c r="B260" s="0" t="s">
         <v>31</v>
@@ -4443,105 +4428,102 @@
         <v>14</v>
       </c>
       <c r="H260" s="0" t="s">
-        <v>64</v>
+        <v>125</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>23</v>
+        <v>163</v>
       </c>
       <c r="B261" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C261" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D261" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E261" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="G261" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H261" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>27</v>
+        <v>164</v>
       </c>
       <c r="B262" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C262" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D262" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E262" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G262" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H262" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B263" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C263" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D263" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E263" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B264" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C264" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D264" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B263" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C263" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D263" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="0" t="s">
+      <c r="B265" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C265" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D265" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="B266" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D266" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E266" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F266" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G266" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H266" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B267" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D267" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E267" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G267" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H267" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="B268" s="0" t="s">
         <v>31</v>
@@ -4552,125 +4534,168 @@
       <c r="E268" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="F268" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="G268" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H268" s="0" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B269" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C269" s="0" t="s">
-        <v>168</v>
+        <v>31</v>
       </c>
       <c r="D269" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E269" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="G269" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H269" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B270" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C270" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D270" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E270" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="G270" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H270" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="B271" s="0" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C271" s="0" t="s">
-        <v>25</v>
+        <v>169</v>
       </c>
       <c r="D271" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E271" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B272" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C272" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D272" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E272" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B273" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C273" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D273" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B272" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C272" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D272" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B275" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C275" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="D275" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E275" s="0" t="s">
-        <v>12</v>
+      <c r="B274" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C274" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D274" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="0" t="s">
+      <c r="A276" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B276" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C276" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="D276" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E276" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B277" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C277" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="D277" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E277" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B278" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C278" s="0" t="n">
+        <v>255</v>
+      </c>
+      <c r="D278" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E278" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B277" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D277" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E277" s="0" t="s">
+      <c r="B279" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D279" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E279" s="0" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
share story under progress
</commit_message>
<xml_diff>
--- a/DB/DB_Schema.xlsx
+++ b/DB/DB_Schema.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="172">
   <si>
     <t xml:space="preserve">Table admin</t>
   </si>
@@ -721,8 +721,8 @@
   </sheetPr>
   <dimension ref="A1:H279"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A144" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C163" activeCellId="0" sqref="C163"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A147" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C178" activeCellId="0" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2355,7 +2355,7 @@
         <v>17</v>
       </c>
       <c r="C115" s="0" t="n">
-        <v>128</v>
+        <v>64</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2366,7 +2366,7 @@
         <v>17</v>
       </c>
       <c r="C116" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2376,8 +2376,8 @@
       <c r="B117" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C117" s="0" t="n">
-        <v>255</v>
+      <c r="C117" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="D117" s="0" t="s">
         <v>18</v>
@@ -2501,7 +2501,7 @@
         <v>17</v>
       </c>
       <c r="C126" s="0" t="n">
-        <v>128</v>
+        <v>64</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2512,7 +2512,7 @@
         <v>17</v>
       </c>
       <c r="C127" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2522,8 +2522,8 @@
       <c r="B128" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C128" s="0" t="n">
-        <v>255</v>
+      <c r="C128" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="D128" s="0" t="s">
         <v>18</v>
@@ -3228,7 +3228,7 @@
         <v>17</v>
       </c>
       <c r="C173" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3238,8 +3238,8 @@
       <c r="B174" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C174" s="0" t="n">
-        <v>255</v>
+      <c r="C174" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="D174" s="0" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
created cms page ui
</commit_message>
<xml_diff>
--- a/DB/DB_Schema.xlsx
+++ b/DB/DB_Schema.xlsx
@@ -724,8 +724,8 @@
   </sheetPr>
   <dimension ref="A1:H282"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A184" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C207" activeCellId="0" sqref="C207"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A208" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B219" activeCellId="0" sqref="B219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3842,7 +3842,7 @@
         <v>17</v>
       </c>
       <c r="C218" s="0" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D218" s="0" t="s">
         <v>11</v>
@@ -3851,7 +3851,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
         <v>81</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>17</v>
       </c>
       <c r="C228" s="0" t="n">
-        <v>255</v>
+        <v>30</v>
       </c>
       <c r="D228" s="0" t="s">
         <v>18</v>

</xml_diff>